<commit_message>
Improved GUI System (Not complete), Changes to Transect Line
</commit_message>
<xml_diff>
--- a/controlbox/Formula.xlsx
+++ b/controlbox/Formula.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\underground\Desktop\SardineROV-master\controlbox\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6167A89C-9669-4219-A6E1-12C8C6CBCAB6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{58927536-DF17-4A83-B15E-00E73495DB65}"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -33,25 +22,368 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -59,33 +391,319 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -97,6 +715,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -110,7 +729,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -122,7 +741,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -158,6 +776,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$21</c:f>
@@ -198,7 +819,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -240,61 +861,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5955190384466475E-3</c:v>
+                  <c:v>0.00259551903844665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.864709984787198E-3</c:v>
+                  <c:v>0.0058647099847872</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9824256652821762E-3</c:v>
+                  <c:v>0.00998242566528218</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5168902290140661E-2</c:v>
+                  <c:v>0.0151689022901407</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1701538797227009E-2</c:v>
+                  <c:v>0.021701538797227</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9929733546852778E-2</c:v>
+                  <c:v>0.0299297335468528</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.029357190894859E-2</c:v>
+                  <c:v>0.0402935719089486</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.334736424906477E-2</c:v>
+                  <c:v>0.0533473642490648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9789293243450956E-2</c:v>
+                  <c:v>0.069789293243451</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0498756211208897E-2</c:v>
+                  <c:v>0.0904987562112089</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.11658339971984903</c:v>
+                  <c:v>0.116583399719849</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.14943836211226599</c:v>
+                  <c:v>0.149438362112266</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.19082089254437976</c:v>
+                  <c:v>0.19082089254438</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.24294433753605826</c:v>
+                  <c:v>0.242944337536058</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30859652191026987</c:v>
+                  <c:v>0.30859652191027</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.39128885573036892</c:v>
+                  <c:v>0.391288855730369</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.49544414222683303</c:v>
+                  <c:v>0.495444142226833</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.62663313162894085</c:v>
+                  <c:v>0.626633131628941</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.79187247299382368</c:v>
+                  <c:v>0.791872472993823</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1</c:v>
@@ -303,11 +924,6 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9D9E-458E-BF20-5309E65C28F6}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -318,7 +934,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -335,6 +951,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$21</c:f>
@@ -375,7 +994,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -417,61 +1036,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.24402745615984E-3</c:v>
+                  <c:v>0.0187447095452885</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3657691278518028E-2</c:v>
+                  <c:v>0.0392462397702631</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2460088714602505E-2</c:v>
+                  <c:v>0.0616692461417432</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2911358488815268E-2</c:v>
+                  <c:v>0.0861938162210511</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5320368725685567E-2</c:v>
+                  <c:v>0.113016916014657</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0053844981239467E-2</c:v>
+                  <c:v>0.142353971881941</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.7547208144724072E-2</c:v>
+                  <c:v>0.174440600704955</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8317442505009928E-2</c:v>
+                  <c:v>0.209534502215844</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1229783742737907</c:v>
+                  <c:v>0.247917528679895</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.15225881209433406</c:v>
+                  <c:v>0.289897948556636</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.18702408564527306</c:v>
+                  <c:v>0.33581292231927</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.22830161887340114</c:v>
+                  <c:v>0.386031210316704</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27731129362549867</c:v>
+                  <c:v>0.440956134426007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.33550150102068288</c:v>
+                  <c:v>0.501028817281439</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.40459194599552251</c:v>
+                  <c:v>0.566731725095527</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.48662447003179782</c:v>
+                  <c:v>0.638592542525895</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.58402339403949077</c:v>
+                  <c:v>0.717188410708359</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.6996671647183178</c:v>
+                  <c:v>0.803150562493524</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.83697342177471834</c:v>
+                  <c:v>0.897169392114193</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1</c:v>
@@ -480,11 +1099,6 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9D9E-458E-BF20-5309E65C28F6}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -495,7 +1109,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>-0.9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -512,6 +1126,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$21</c:f>
@@ -552,7 +1169,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -594,61 +1211,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5264923841377582E-2</c:v>
+                  <c:v>0.120832290962505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1773462536293131E-2</c:v>
+                  <c:v>0.228524183639687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10956947206784506</c:v>
+                  <c:v>0.324504684017625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1486983549970351</c:v>
+                  <c:v>0.410047395022008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18920711500272103</c:v>
+                  <c:v>0.486287416455168</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23114441334491631</c:v>
+                  <c:v>0.554236407080809</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.27456062731926201</c:v>
+                  <c:v>0.614796008721152</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3195079107728942</c:v>
+                  <c:v>0.668769810496114</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36604025675439544</c:v>
+                  <c:v>0.716874011962694</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.41421356237309515</c:v>
+                  <c:v>0.759746926647958</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.46408569594562543</c:v>
+                  <c:v>0.797957452081727</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.51571656651039799</c:v>
+                  <c:v>0.832012618721158</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.56916819579350153</c:v>
+                  <c:v>0.862364317936851</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.62450479271247095</c:v>
+                  <c:v>0.889415298336791</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.681792830507429</c:v>
+                  <c:v>0.913524509995675</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.74110112659224825</c:v>
+                  <c:v>0.935011867504321</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.80250092522166039</c:v>
+                  <c:v>0.954162495041916</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.86606598307361482</c:v>
+                  <c:v>0.971230509800648</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.93187265784969098</c:v>
+                  <c:v>0.986442393966449</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1</c:v>
@@ -657,11 +1274,6 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9D9E-458E-BF20-5309E65C28F6}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -672,7 +1284,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-0.999</c:v>
+                  <c:v>0.005</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -689,6 +1301,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$21</c:f>
@@ -729,7 +1344,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -771,74 +1386,69 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29234656217804017</c:v>
+                  <c:v>0.0498816345199327</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49931207845117886</c:v>
+                  <c:v>0.0997757099272079</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64583244320963407</c:v>
+                  <c:v>0.149682229324632</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74956091776680889</c:v>
+                  <c:v>0.199601195815902</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82299505405015794</c:v>
+                  <c:v>0.249532612505332</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87498244126184521</c:v>
+                  <c:v>0.299476482498173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.91178669287950498</c:v>
+                  <c:v>0.349432808900385</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93784210765964038</c:v>
+                  <c:v>0.399401594818638</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95628792871361734</c:v>
+                  <c:v>0.449382843360491</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.96934656996828461</c:v>
+                  <c:v>0.499376557634212</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.97859137999431089</c:v>
+                  <c:v>0.549382740748827</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.98513620427966864</c:v>
+                  <c:v>0.599401395814203</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.9897695850420225</c:v>
+                  <c:v>0.649432525940963</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.99304976742017748</c:v>
+                  <c:v>0.69947613424044</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.99537195870680339</c:v>
+                  <c:v>0.749532223824811</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.99701594423870388</c:v>
+                  <c:v>0.79960079780701</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99817979686560121</c:v>
+                  <c:v>0.849681859300722</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99900374142645776</c:v>
+                  <c:v>0.899775411420523</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.9995870495048822</c:v>
+                  <c:v>0.949881457281565</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>0.999999999999979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-9D9E-458E-BF20-5309E65C28F6}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -848,6 +1458,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="0"/>
         <c:smooth val="0"/>
         <c:axId val="529190448"/>
         <c:axId val="441286704"/>
@@ -881,7 +1492,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -893,7 +1504,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="441286704"/>
@@ -940,7 +1550,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -952,7 +1562,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="529190448"/>
@@ -969,6 +1578,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -982,7 +1592,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -994,19 +1604,11 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1029,9 +1631,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="zh-CN"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1599,7 +2200,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -1613,20 +2214,14 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B3C46F6-CE41-4E63-95FC-D070B8D34B24}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="6705600" y="796290"/>
+        <a:ext cx="4632960" cy="3831590"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1682,7 +2277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1715,26 +2310,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1767,23 +2345,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1925,39 +2486,34 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAECF18-FEA8-412D-8864-DCC003A5FD5A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <f>1/B$24*( (B$24+1)^A1 - 1)</f>
+        <f>1/B$24*((B$24+1)^A1-1)</f>
         <v>0</v>
       </c>
       <c r="C1">
-        <f>1/C$24*( (C$24+1)^B1 - 1)</f>
+        <f>1/C$24*((C$24+1)^B1-1)</f>
         <v>0</v>
       </c>
       <c r="D1">
-        <f t="shared" ref="D1:E1" si="0">1/D$24*( (D$24+1)^C1 - 1)</f>
+        <f t="shared" ref="D1:E1" si="0">1/D$24*((D$24+1)^C1-1)</f>
         <v>0</v>
       </c>
       <c r="E1">
@@ -1965,406 +2521,406 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0.05</v>
       </c>
       <c r="B2">
-        <f>1/B$24*( (B$24+1)^$A2 - 1)</f>
-        <v>2.5955190384466475E-3</v>
+        <f>1/B$24*((B$24+1)^$A2-1)</f>
+        <v>0.00259551903844665</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:E2" si="1">1/C$24*( (C$24+1)^$A2 - 1)</f>
-        <v>6.24402745615984E-3</v>
+        <f t="shared" ref="C2:E2" si="1">1/C$24*((C$24+1)^$A2-1)</f>
+        <v>0.0187447095452885</v>
       </c>
       <c r="D2">
         <f t="shared" si="1"/>
-        <v>3.5264923841377582E-2</v>
+        <v>0.120832290962505</v>
       </c>
       <c r="E2">
         <f t="shared" si="1"/>
-        <v>0.29234656217804017</v>
+        <v>0.0498816345199327</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>0.1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:E21" si="2">1/B$24*( (B$24+1)^$A3 - 1)</f>
-        <v>5.864709984787198E-3</v>
+        <f t="shared" ref="B3:E21" si="2">1/B$24*((B$24+1)^$A3-1)</f>
+        <v>0.0058647099847872</v>
       </c>
       <c r="C3">
         <f t="shared" si="2"/>
-        <v>1.3657691278518028E-2</v>
+        <v>0.0392462397702631</v>
       </c>
       <c r="D3">
         <f t="shared" si="2"/>
-        <v>7.1773462536293131E-2</v>
+        <v>0.228524183639687</v>
       </c>
       <c r="E3">
         <f t="shared" si="2"/>
-        <v>0.49931207845117886</v>
+        <v>0.0997757099272079</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>0.15</v>
       </c>
       <c r="B4">
         <f t="shared" si="2"/>
-        <v>9.9824256652821762E-3</v>
+        <v>0.00998242566528218</v>
       </c>
       <c r="C4">
         <f t="shared" si="2"/>
-        <v>2.2460088714602505E-2</v>
+        <v>0.0616692461417432</v>
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
-        <v>0.10956947206784506</v>
+        <v>0.324504684017625</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>0.64583244320963407</v>
+        <v>0.149682229324632</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>0.2</v>
       </c>
       <c r="B5">
         <f t="shared" si="2"/>
-        <v>1.5168902290140661E-2</v>
+        <v>0.0151689022901407</v>
       </c>
       <c r="C5">
         <f t="shared" si="2"/>
-        <v>3.2911358488815268E-2</v>
+        <v>0.0861938162210511</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>0.1486983549970351</v>
+        <v>0.410047395022008</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>0.74956091776680889</v>
+        <v>0.199601195815902</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>0.25</v>
       </c>
       <c r="B6">
         <f t="shared" si="2"/>
-        <v>2.1701538797227009E-2</v>
+        <v>0.021701538797227</v>
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
-        <v>4.5320368725685567E-2</v>
+        <v>0.113016916014657</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>0.18920711500272103</v>
+        <v>0.486287416455168</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>0.82299505405015794</v>
+        <v>0.249532612505332</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>0.3</v>
       </c>
       <c r="B7">
         <f t="shared" si="2"/>
-        <v>2.9929733546852778E-2</v>
+        <v>0.0299297335468528</v>
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
-        <v>6.0053844981239467E-2</v>
+        <v>0.142353971881941</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>0.23114441334491631</v>
+        <v>0.554236407080809</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>0.87498244126184521</v>
+        <v>0.299476482498173</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>0.35</v>
       </c>
       <c r="B8">
         <f t="shared" si="2"/>
-        <v>4.029357190894859E-2</v>
+        <v>0.0402935719089486</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
-        <v>7.7547208144724072E-2</v>
+        <v>0.174440600704955</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>0.27456062731926201</v>
+        <v>0.614796008721152</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>0.91178669287950498</v>
+        <v>0.349432808900385</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>0.4</v>
       </c>
       <c r="B9">
         <f t="shared" si="2"/>
-        <v>5.334736424906477E-2</v>
+        <v>0.0533473642490648</v>
       </c>
       <c r="C9">
         <f t="shared" si="2"/>
-        <v>9.8317442505009928E-2</v>
+        <v>0.209534502215844</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>0.3195079107728942</v>
+        <v>0.668769810496114</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>0.93784210765964038</v>
+        <v>0.399401594818638</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>0.45</v>
       </c>
       <c r="B10">
         <f t="shared" si="2"/>
-        <v>6.9789293243450956E-2</v>
+        <v>0.069789293243451</v>
       </c>
       <c r="C10">
         <f t="shared" si="2"/>
-        <v>0.1229783742737907</v>
+        <v>0.247917528679895</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>0.36604025675439544</v>
+        <v>0.716874011962694</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>0.95628792871361734</v>
+        <v>0.449382843360491</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>0.5</v>
       </c>
       <c r="B11">
         <f t="shared" si="2"/>
-        <v>9.0498756211208897E-2</v>
+        <v>0.0904987562112089</v>
       </c>
       <c r="C11">
         <f t="shared" si="2"/>
-        <v>0.15225881209433406</v>
+        <v>0.289897948556636</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>0.41421356237309515</v>
+        <v>0.759746926647958</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>0.96934656996828461</v>
+        <v>0.499376557634212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="B12">
         <f t="shared" si="2"/>
-        <v>0.11658339971984903</v>
+        <v>0.116583399719849</v>
       </c>
       <c r="C12">
         <f t="shared" si="2"/>
-        <v>0.18702408564527306</v>
+        <v>0.33581292231927</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>0.46408569594562543</v>
+        <v>0.797957452081727</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>0.97859137999431089</v>
+        <v>0.549382740748827</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>0.6</v>
       </c>
       <c r="B13">
         <f t="shared" si="2"/>
-        <v>0.14943836211226599</v>
+        <v>0.149438362112266</v>
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
-        <v>0.22830161887340114</v>
+        <v>0.386031210316704</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>0.51571656651039799</v>
+        <v>0.832012618721158</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>0.98513620427966864</v>
+        <v>0.599401395814203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>0.65</v>
       </c>
       <c r="B14">
         <f t="shared" si="2"/>
-        <v>0.19082089254437976</v>
+        <v>0.19082089254438</v>
       </c>
       <c r="C14">
         <f t="shared" si="2"/>
-        <v>0.27731129362549867</v>
+        <v>0.440956134426007</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>0.56916819579350153</v>
+        <v>0.862364317936851</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0.9897695850420225</v>
+        <v>0.649432525940963</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>0.7</v>
       </c>
       <c r="B15">
         <f t="shared" si="2"/>
-        <v>0.24294433753605826</v>
+        <v>0.242944337536058</v>
       </c>
       <c r="C15">
         <f t="shared" si="2"/>
-        <v>0.33550150102068288</v>
+        <v>0.501028817281439</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>0.62450479271247095</v>
+        <v>0.889415298336791</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>0.99304976742017748</v>
+        <v>0.69947613424044</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>0.75</v>
       </c>
       <c r="B16">
         <f t="shared" si="2"/>
-        <v>0.30859652191026987</v>
+        <v>0.30859652191027</v>
       </c>
       <c r="C16">
         <f t="shared" si="2"/>
-        <v>0.40459194599552251</v>
+        <v>0.566731725095527</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>0.681792830507429</v>
+        <v>0.913524509995675</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>0.99537195870680339</v>
+        <v>0.749532223824811</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>0.8</v>
       </c>
       <c r="B17">
         <f t="shared" si="2"/>
-        <v>0.39128885573036892</v>
+        <v>0.391288855730369</v>
       </c>
       <c r="C17">
         <f t="shared" si="2"/>
-        <v>0.48662447003179782</v>
+        <v>0.638592542525895</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>0.74110112659224825</v>
+        <v>0.935011867504321</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>0.99701594423870388</v>
+        <v>0.79960079780701</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>0.85</v>
       </c>
       <c r="B18">
         <f t="shared" si="2"/>
-        <v>0.49544414222683303</v>
+        <v>0.495444142226833</v>
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
-        <v>0.58402339403949077</v>
+        <v>0.717188410708359</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>0.80250092522166039</v>
+        <v>0.954162495041916</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>0.99817979686560121</v>
+        <v>0.849681859300722</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>0.9</v>
       </c>
       <c r="B19">
         <f t="shared" si="2"/>
-        <v>0.62663313162894085</v>
+        <v>0.626633131628941</v>
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
-        <v>0.6996671647183178</v>
+        <v>0.803150562493524</v>
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>0.86606598307361482</v>
+        <v>0.971230509800648</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>0.99900374142645776</v>
+        <v>0.899775411420523</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>0.95</v>
       </c>
       <c r="B20">
         <f t="shared" si="2"/>
-        <v>0.79187247299382368</v>
+        <v>0.791872472993823</v>
       </c>
       <c r="C20">
         <f t="shared" si="2"/>
-        <v>0.83697342177471834</v>
+        <v>0.897169392114193</v>
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>0.93187265784969098</v>
+        <v>0.986442393966449</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>0.9995870495048822</v>
+        <v>0.949881457281565</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2382,10 +2938,10 @@
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.999999999999979</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2393,17 +2949,18 @@
         <v>100</v>
       </c>
       <c r="C24">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>-0.9</v>
       </c>
       <c r="E24">
-        <v>-0.999</v>
+        <v>0.005</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>